<commit_message>
1. Refactoring Tool Final update.
Signed-off-by: sm67nono <manna.subhadeep@gmail.com>
</commit_message>
<xml_diff>
--- a/Report/Refactoring_Functional2Iterative_Consolidated.xlsx
+++ b/Report/Refactoring_Functional2Iterative_Consolidated.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="38">
   <si>
     <t>Filter</t>
   </si>
@@ -147,9 +147,6 @@
   </si>
   <si>
     <t>54.20s</t>
-  </si>
-  <si>
-    <t>7/15=0.46</t>
   </si>
   <si>
     <t>7/15=0.47</t>
@@ -657,7 +654,7 @@
   <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1172,7 +1169,7 @@
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -1185,7 +1182,7 @@
   <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>